<commit_message>
Bài 29 - DataProvider
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UsersData.xlsx
+++ b/src/test/resources/testdata/UsersData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_042023\SeleniumTestNGParallel042023\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C509707C-1E7B-4C02-BC90-026413AB4150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1066BF67-FD3B-47B7-9772-19F6ADA5B64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4656" yWindow="2028" windowWidth="22704" windowHeight="13872" xr2:uid="{9C3794C8-DDC7-4EBF-8496-CA116BCAD0C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9C3794C8-DDC7-4EBF-8496-CA116BCAD0C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>